<commit_message>
add UC alpha (1.3.1), chờ thầy xác nhận
</commit_message>
<xml_diff>
--- a/Docs/PLAN/DD_RFID_CM_v1.0.xlsx
+++ b/Docs/PLAN/DD_RFID_CM_v1.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8130" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lịch sử thay đổi" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
     <r>
       <t>*A - Add</t>
@@ -161,9 +161,6 @@
     <t>Tên các tài liệu:</t>
   </si>
   <si>
-    <t>DD_RFID_&lt;tên viết tắt tài liệu&gt;_v&lt;số phiên bản&gt;</t>
-  </si>
-  <si>
     <t>Chú giải:</t>
   </si>
   <si>
@@ -279,6 +276,12 @@
   </si>
   <si>
     <t>Lưu các tài liệu ghi chú khi gặp và trao đổi với GV hướng dẫn</t>
+  </si>
+  <si>
+    <t>DD_RFID_&lt;tên viết tắt tài liệu&gt;_v&lt;số phiên bản&gt;[_alpha|_beta|_Realease]</t>
+  </si>
+  <si>
+    <t>DD_RIFD_ScreenDesign_v1.0_beta</t>
   </si>
 </sst>
 </file>
@@ -1734,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,42 +1765,42 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1805,28 +1808,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B20" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -1841,10 +1833,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12" t="s">
-        <v>13</v>
-      </c>
+      <c r="B21" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -1858,7 +1850,9 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
+      <c r="C22" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -1871,9 +1865,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="B23" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
@@ -1887,10 +1879,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12" t="s">
-        <v>13</v>
-      </c>
+      <c r="B24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1904,7 +1896,9 @@
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
+      <c r="C25" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -1917,9 +1911,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
-      <c r="B26" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
@@ -1933,10 +1925,10 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12" t="s">
-        <v>13</v>
-      </c>
+      <c r="B27" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -1950,7 +1942,9 @@
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+      <c r="C28" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
@@ -1962,12 +1956,8 @@
       <c r="L28" s="12"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
@@ -1980,9 +1970,11 @@
       <c r="L29" s="12"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+      <c r="A30" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="B30" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
@@ -1997,10 +1989,10 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="B31" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -2014,7 +2006,9 @@
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
+      <c r="C32" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
@@ -2027,9 +2021,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
-      <c r="B33" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
@@ -2043,10 +2035,10 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="B34" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -2061,7 +2053,7 @@
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
@@ -2077,7 +2069,7 @@
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
@@ -2092,7 +2084,9 @@
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
+      <c r="C37" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
@@ -2105,9 +2099,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
-      <c r="B38" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
@@ -2121,10 +2113,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12" t="s">
-        <v>22</v>
-      </c>
+      <c r="B39" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
@@ -2138,10 +2130,10 @@
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="C40" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
@@ -2150,6 +2142,22 @@
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2163,8 +2171,8 @@
   </sheetPr>
   <dimension ref="A1:BG26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2183,7 @@
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2239,7 +2247,7 @@
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -2302,7 +2310,7 @@
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -2428,7 +2436,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -2492,7 +2500,7 @@
       <c r="A6" s="14"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -2556,7 +2564,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2680,7 +2688,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -2804,7 +2812,7 @@
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
@@ -2819,7 +2827,7 @@
       <c r="M11" s="22"/>
       <c r="N11" s="23"/>
       <c r="O11" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P11" s="22"/>
       <c r="Q11" s="22"/>
@@ -2843,7 +2851,7 @@
       <c r="B12" s="24"/>
       <c r="C12" s="25"/>
       <c r="D12" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
@@ -2856,7 +2864,7 @@
       <c r="M12" s="27"/>
       <c r="N12" s="25"/>
       <c r="O12" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P12" s="27"/>
       <c r="Q12" s="27"/>
@@ -2881,7 +2889,7 @@
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
@@ -2917,7 +2925,7 @@
       <c r="D14" s="30"/>
       <c r="E14" s="29"/>
       <c r="F14" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="29"/>
       <c r="H14" s="29"/>
@@ -2928,7 +2936,7 @@
       <c r="M14" s="29"/>
       <c r="N14" s="30"/>
       <c r="O14" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P14" s="29"/>
       <c r="Q14" s="29"/>
@@ -2954,7 +2962,7 @@
       <c r="D15" s="30"/>
       <c r="E15" s="29"/>
       <c r="F15" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2965,7 +2973,7 @@
       <c r="M15" s="29"/>
       <c r="N15" s="30"/>
       <c r="O15" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P15" s="29"/>
       <c r="Q15" s="29"/>
@@ -2991,7 +2999,7 @@
       <c r="D16" s="30"/>
       <c r="E16" s="29"/>
       <c r="F16" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
@@ -3002,7 +3010,7 @@
       <c r="M16" s="29"/>
       <c r="N16" s="30"/>
       <c r="O16" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
@@ -3028,7 +3036,7 @@
       <c r="D17" s="30"/>
       <c r="E17" s="29"/>
       <c r="F17" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G17" s="29"/>
       <c r="H17" s="29"/>
@@ -3039,7 +3047,7 @@
       <c r="M17" s="29"/>
       <c r="N17" s="30"/>
       <c r="O17" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P17" s="29"/>
       <c r="Q17" s="29"/>
@@ -3065,7 +3073,7 @@
       <c r="D18" s="30"/>
       <c r="E18" s="29"/>
       <c r="F18" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" s="29"/>
       <c r="H18" s="29"/>
@@ -3076,7 +3084,7 @@
       <c r="M18" s="29"/>
       <c r="N18" s="30"/>
       <c r="O18" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P18" s="29"/>
       <c r="Q18" s="29"/>
@@ -3102,7 +3110,7 @@
       <c r="D19" s="30"/>
       <c r="E19" s="29"/>
       <c r="F19" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G19" s="29"/>
       <c r="H19" s="29"/>
@@ -3113,7 +3121,7 @@
       <c r="M19" s="29"/>
       <c r="N19" s="30"/>
       <c r="O19" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P19" s="29"/>
       <c r="Q19" s="29"/>
@@ -3139,7 +3147,7 @@
       <c r="D20" s="30"/>
       <c r="E20" s="29"/>
       <c r="F20" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G20" s="29"/>
       <c r="H20" s="29"/>
@@ -3175,7 +3183,7 @@
       <c r="E21" s="28"/>
       <c r="F21" s="29"/>
       <c r="G21" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
@@ -3185,7 +3193,7 @@
       <c r="M21" s="29"/>
       <c r="N21" s="30"/>
       <c r="O21" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P21" s="29"/>
       <c r="Q21" s="29"/>
@@ -3210,7 +3218,7 @@
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
       <c r="E22" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
@@ -3222,7 +3230,7 @@
       <c r="M22" s="29"/>
       <c r="N22" s="30"/>
       <c r="O22" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P22" s="29"/>
       <c r="Q22" s="29"/>
@@ -3247,7 +3255,7 @@
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
       <c r="E23" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
@@ -3259,7 +3267,7 @@
       <c r="M23" s="29"/>
       <c r="N23" s="30"/>
       <c r="O23" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P23" s="29"/>
       <c r="Q23" s="29"/>

</xml_diff>